<commit_message>
finalise modularisation for fatigue module, update alignment table and deleted-classes file
</commit_message>
<xml_diff>
--- a/alignments.xlsx
+++ b/alignments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="165">
   <si>
     <t>concept in mechanical testing ontology</t>
   </si>
@@ -498,6 +498,27 @@
   </si>
   <si>
     <t>based on EMMO version</t>
+  </si>
+  <si>
+    <t>http://emmo.info/emmo/domain/mechanical-testing#EMMO_16d31733_248f_4e55_b870_dfc96d3e2c3b</t>
+  </si>
+  <si>
+    <t>DataSet</t>
+  </si>
+  <si>
+    <t>Series</t>
+  </si>
+  <si>
+    <t>SymbolicConstruct</t>
+  </si>
+  <si>
+    <t>http://emmo.info/emmo#EMMO_194e367c_9783_4bf5_96d0_9ad597d48d9a</t>
+  </si>
+  <si>
+    <t>EMMO/perspectives/data</t>
+  </si>
+  <si>
+    <t>beta4</t>
   </si>
 </sst>
 </file>
@@ -625,6 +646,12 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -634,12 +661,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -924,7 +945,7 @@
   <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -939,46 +960,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="2" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="7" t="s">
         <v>157</v>
       </c>
     </row>
@@ -1128,60 +1149,60 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="7" t="s">
+      <c r="C8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="I8" s="7" t="s">
+      <c r="H8" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="7" t="s">
+      <c r="C9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>75</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="I9" s="7" t="s">
+      <c r="H9" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1566,7 +1587,7 @@
       <c r="A23" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C23" t="s">
@@ -1595,7 +1616,7 @@
       <c r="A24" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C24" t="s">
@@ -1624,7 +1645,7 @@
       <c r="A25" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C25" t="s">
@@ -1682,7 +1703,7 @@
       <c r="A27" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C27" t="s">
@@ -1842,7 +1863,7 @@
       <c r="F32" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G32" s="3" t="s">
         <v>111</v>
       </c>
       <c r="H32" t="s">
@@ -1885,7 +1906,7 @@
       <c r="A34" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C34" t="s">
@@ -1940,7 +1961,33 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F36" s="1"/>
+      <c r="A36" t="s">
+        <v>159</v>
+      </c>
+      <c r="B36" t="s">
+        <v>158</v>
+      </c>
+      <c r="C36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" t="s">
+        <v>160</v>
+      </c>
+      <c r="E36" t="s">
+        <v>161</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G36" t="s">
+        <v>162</v>
+      </c>
+      <c r="H36" t="s">
+        <v>163</v>
+      </c>
+      <c r="I36" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F37" s="1"/>
@@ -1964,46 +2011,46 @@
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F44" s="8"/>
+      <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="4"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="2" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="2" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="58" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
     </row>
     <row r="59" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E59" s="7"/>
-      <c r="F59" s="7"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
     </row>
     <row r="60" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E60" s="7"/>
+      <c r="E60" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Finalise Fatigue Module: recreate relations that had been removed during the modularisation process, set 'FatigueUseCase' as rootclass for all concepts in the Fatigue Module.
</commit_message>
<xml_diff>
--- a/alignments.xlsx
+++ b/alignments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="186">
   <si>
     <t>concept in mechanical testing ontology</t>
   </si>
@@ -519,6 +519,69 @@
   </si>
   <si>
     <t>beta4</t>
+  </si>
+  <si>
+    <t>In Fatigue module:</t>
+  </si>
+  <si>
+    <t>Revise Failure concepts:</t>
+  </si>
+  <si>
+    <t>FailureComment, FailureOrigin, FailureReason (subclasses Featureless, Inclusion (subclass InclusionElements), Pore, FailureType (subclasses: SurfaceFailure, VolumeFailure)</t>
+  </si>
+  <si>
+    <t>Fractography</t>
+  </si>
+  <si>
+    <t>Currently has superclass "Measurement", but isnt it a method, and a FractographyMeasurement is the measurement itself?</t>
+  </si>
+  <si>
+    <t>…revise all concepts for suitability as subclasses of:</t>
+  </si>
+  <si>
+    <t>Device [from oie/manufacturing]</t>
+  </si>
+  <si>
+    <t>Characterisation Machine [chameo]</t>
+  </si>
+  <si>
+    <t>Detector [chameo]</t>
+  </si>
+  <si>
+    <t>"Calibration Data" [chameo]</t>
+  </si>
+  <si>
+    <t>"Primary Data" [chameo]</t>
+  </si>
+  <si>
+    <t>"Raw Data" [chameo]</t>
+  </si>
+  <si>
+    <t>"Secondary Data" [chameo]</t>
+  </si>
+  <si>
+    <t>"Characterisation Property" [chameo]</t>
+  </si>
+  <si>
+    <t>…"Device" is double, 1x from oie/manufacturing and 1x from emmo beta4, the classes have different meanings, IRIs, and subclasses, but the same label.</t>
+  </si>
+  <si>
+    <t>same as Fractography</t>
+  </si>
+  <si>
+    <t>FatigueTesting and subclasses</t>
+  </si>
+  <si>
+    <t>"Characterisation Method" [chameo]</t>
+  </si>
+  <si>
+    <t>"Measurement Process" [chameo]</t>
+  </si>
+  <si>
+    <t>"Calibration Measurement" [chameo]</t>
+  </si>
+  <si>
+    <t>"Characterisation Workflow" [chameo]</t>
   </si>
 </sst>
 </file>
@@ -1061,10 +1124,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2217,24 +2280,129 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>150</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="58" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-    </row>
-    <row r="59" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-    </row>
-    <row r="60" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E60" s="2"/>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="1"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B67" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B68" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B69" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E76" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Finalise Mechanical Testing Module: set 'MechanicalTestingOntology' as rootclass for all concepts in this module, update open tasks in alignments.xlsx
</commit_message>
<xml_diff>
--- a/alignments.xlsx
+++ b/alignments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="194">
   <si>
     <t>concept in mechanical testing ontology</t>
   </si>
@@ -582,6 +582,30 @@
   </si>
   <si>
     <t>"Characterisation Workflow" [chameo]</t>
+  </si>
+  <si>
+    <t>In Mechanical testing module:</t>
+  </si>
+  <si>
+    <t>CantileverBending and TwoPointBending</t>
+  </si>
+  <si>
+    <t>are subclasses of BendingMeasurement -&gt; but aren't they methods, and for the measurement process itself it should be, e.g., CantileverBendingMeasurement?</t>
+  </si>
+  <si>
+    <t>MechanicalTesting</t>
+  </si>
+  <si>
+    <t>TensileTesting</t>
+  </si>
+  <si>
+    <t>same as CantileverBending</t>
+  </si>
+  <si>
+    <t>TensileTestMeasurement</t>
+  </si>
+  <si>
+    <t>exists, but what is the difference to TensileTesting, and why are they both a "Measurement"?</t>
   </si>
 </sst>
 </file>
@@ -1124,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I76"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2284,125 +2308,177 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>150</v>
-      </c>
+      <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="1"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="1"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="1"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B70" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B71" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B72" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B73" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="1"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B77" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B78" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B79" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E76" s="2"/>
+    <row r="84" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+    </row>
+    <row r="85" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+    </row>
+    <row r="86" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E86" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>